<commit_message>
Fixed some of the bugs, made the plots a little better, and wrote all the supporting information for submission
</commit_message>
<xml_diff>
--- a/flashdrive/Growth_Curves/Nanobody_Library_ConditionTest_1.xlsx
+++ b/flashdrive/Growth_Curves/Nanobody_Library_ConditionTest_1.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CodyCole/Desktop/CSB_CodingProject/flashdrive/Growth_Curves/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53D32AB-B1E0-5245-9A07-D852AAEFF7F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="1120" windowWidth="24480" windowHeight="17260" tabRatio="500"/>
+    <workbookView xWindow="1120" yWindow="460" windowWidth="24480" windowHeight="14600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -318,7 +324,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -358,6 +364,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -682,16 +696,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CT42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:CT42"/>
+    <sheetView tabSelected="1" topLeftCell="BH1" workbookViewId="0">
+      <selection activeCell="CT2" sqref="CT2:CT42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:98">
+    <row r="1" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -987,7 +1001,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:98">
+    <row r="2" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1241,10 +1255,10 @@
         <v>9.4100000000000003E-2</v>
       </c>
       <c r="CG2">
-        <v>9.5500000000000002E-2</v>
+        <v>9.4100000000000003E-2</v>
       </c>
       <c r="CH2">
-        <v>9.6100000000000005E-2</v>
+        <v>9.4100000000000003E-2</v>
       </c>
       <c r="CI2">
         <v>0.10199999999999999</v>
@@ -1277,13 +1291,13 @@
         <v>9.7799999999999998E-2</v>
       </c>
       <c r="CS2">
-        <v>9.7100000000000006E-2</v>
+        <v>9.4100000000000003E-2</v>
       </c>
       <c r="CT2">
-        <v>9.7900000000000001E-2</v>
+        <v>9.4100000000000003E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:98">
+    <row r="3" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1537,10 +1551,10 @@
         <v>9.4E-2</v>
       </c>
       <c r="CG3">
-        <v>9.5299999999999996E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="CH3">
-        <v>9.5100000000000004E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="CI3">
         <v>9.9199999999999997E-2</v>
@@ -1573,13 +1587,13 @@
         <v>9.7500000000000003E-2</v>
       </c>
       <c r="CS3">
-        <v>9.6699999999999994E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="CT3">
-        <v>9.8799999999999999E-2</v>
+        <v>9.4E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:98">
+    <row r="4" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1833,10 +1847,10 @@
         <v>9.3899999999999997E-2</v>
       </c>
       <c r="CG4">
-        <v>9.5200000000000007E-2</v>
+        <v>9.3899999999999997E-2</v>
       </c>
       <c r="CH4">
-        <v>9.4600000000000004E-2</v>
+        <v>9.3899999999999997E-2</v>
       </c>
       <c r="CI4">
         <v>0.1008</v>
@@ -1869,13 +1883,13 @@
         <v>9.74E-2</v>
       </c>
       <c r="CS4">
-        <v>9.6600000000000005E-2</v>
+        <v>9.3899999999999997E-2</v>
       </c>
       <c r="CT4">
-        <v>9.9099999999999994E-2</v>
+        <v>9.3899999999999997E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:98">
+    <row r="5" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3.125E-2</v>
       </c>
@@ -2129,10 +2143,10 @@
         <v>9.4E-2</v>
       </c>
       <c r="CG5">
-        <v>9.5200000000000007E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="CH5">
-        <v>9.5399999999999999E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="CI5">
         <v>0.1041</v>
@@ -2165,13 +2179,13 @@
         <v>9.7299999999999998E-2</v>
       </c>
       <c r="CS5">
-        <v>9.69E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="CT5">
-        <v>9.9199999999999997E-2</v>
+        <v>9.4E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:98">
+    <row r="6" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -2425,10 +2439,10 @@
         <v>9.3899999999999997E-2</v>
       </c>
       <c r="CG6">
-        <v>9.5100000000000004E-2</v>
+        <v>9.3899999999999997E-2</v>
       </c>
       <c r="CH6">
-        <v>9.5200000000000007E-2</v>
+        <v>9.3899999999999997E-2</v>
       </c>
       <c r="CI6">
         <v>0.1103</v>
@@ -2461,13 +2475,13 @@
         <v>9.7299999999999998E-2</v>
       </c>
       <c r="CS6">
-        <v>0.1012</v>
+        <v>9.3899999999999997E-2</v>
       </c>
       <c r="CT6">
-        <v>9.9400000000000002E-2</v>
+        <v>9.3899999999999997E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:98">
+    <row r="7" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5.2083333333333336E-2</v>
       </c>
@@ -2721,10 +2735,10 @@
         <v>9.4399999999999998E-2</v>
       </c>
       <c r="CG7">
-        <v>9.5500000000000002E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
       <c r="CH7">
-        <v>9.5600000000000004E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
       <c r="CI7">
         <v>0.1216</v>
@@ -2757,13 +2771,13 @@
         <v>9.7900000000000001E-2</v>
       </c>
       <c r="CS7">
-        <v>9.7699999999999995E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
       <c r="CT7">
-        <v>9.98E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:98">
+    <row r="8" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6.25E-2</v>
       </c>
@@ -3017,10 +3031,10 @@
         <v>9.4399999999999998E-2</v>
       </c>
       <c r="CG8">
-        <v>9.5600000000000004E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
       <c r="CH8">
-        <v>9.5600000000000004E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
       <c r="CI8">
         <v>0.1386</v>
@@ -3053,13 +3067,13 @@
         <v>9.7900000000000001E-2</v>
       </c>
       <c r="CS8">
-        <v>9.8100000000000007E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
       <c r="CT8">
-        <v>9.9900000000000003E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:98">
+    <row r="9" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7.2916666666666671E-2</v>
       </c>
@@ -3313,10 +3327,10 @@
         <v>9.4399999999999998E-2</v>
       </c>
       <c r="CG9">
-        <v>9.5500000000000002E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
       <c r="CH9">
-        <v>9.5000000000000001E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
       <c r="CI9">
         <v>0.16750000000000001</v>
@@ -3349,13 +3363,13 @@
         <v>9.7699999999999995E-2</v>
       </c>
       <c r="CS9">
-        <v>9.9500000000000005E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
       <c r="CT9">
-        <v>9.9299999999999999E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:98">
+    <row r="10" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
@@ -3609,10 +3623,10 @@
         <v>9.4399999999999998E-2</v>
       </c>
       <c r="CG10">
-        <v>9.5500000000000002E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
       <c r="CH10">
-        <v>9.5500000000000002E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
       <c r="CI10">
         <v>0.21510000000000001</v>
@@ -3645,13 +3659,13 @@
         <v>9.7799999999999998E-2</v>
       </c>
       <c r="CS10">
-        <v>9.7000000000000003E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
       <c r="CT10">
-        <v>9.9599999999999994E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:98">
+    <row r="11" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9.375E-2</v>
       </c>
@@ -3905,10 +3919,10 @@
         <v>9.4399999999999998E-2</v>
       </c>
       <c r="CG11">
-        <v>9.5399999999999999E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
       <c r="CH11">
-        <v>9.5000000000000001E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
       <c r="CI11">
         <v>0.27650000000000002</v>
@@ -3941,13 +3955,13 @@
         <v>9.7699999999999995E-2</v>
       </c>
       <c r="CS11">
-        <v>9.9500000000000005E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
       <c r="CT11">
-        <v>9.9299999999999999E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:98">
+    <row r="12" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>0.10416666666666667</v>
       </c>
@@ -4201,10 +4215,10 @@
         <v>9.4399999999999998E-2</v>
       </c>
       <c r="CG12">
-        <v>9.5399999999999999E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
       <c r="CH12">
-        <v>9.5000000000000001E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
       <c r="CI12">
         <v>0.36919999999999997</v>
@@ -4237,13 +4251,13 @@
         <v>9.7799999999999998E-2</v>
       </c>
       <c r="CS12">
-        <v>9.9299999999999999E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
       <c r="CT12">
-        <v>9.9500000000000005E-2</v>
+        <v>9.4399999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:98">
+    <row r="13" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>0.11458333333333333</v>
       </c>
@@ -4497,10 +4511,10 @@
         <v>9.4200000000000006E-2</v>
       </c>
       <c r="CG13">
-        <v>9.5899999999999999E-2</v>
+        <v>9.4200000000000006E-2</v>
       </c>
       <c r="CH13">
-        <v>9.5299999999999996E-2</v>
+        <v>9.4200000000000006E-2</v>
       </c>
       <c r="CI13">
         <v>0.48570000000000002</v>
@@ -4533,13 +4547,13 @@
         <v>9.7600000000000006E-2</v>
       </c>
       <c r="CS13">
-        <v>9.9900000000000003E-2</v>
+        <v>9.4200000000000006E-2</v>
       </c>
       <c r="CT13">
-        <v>0.1014</v>
+        <v>9.4200000000000006E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:98">
+    <row r="14" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>0.125</v>
       </c>
@@ -4793,10 +4807,10 @@
         <v>9.4200000000000006E-2</v>
       </c>
       <c r="CG14">
-        <v>9.5100000000000004E-2</v>
+        <v>9.4200000000000006E-2</v>
       </c>
       <c r="CH14">
-        <v>9.5299999999999996E-2</v>
+        <v>9.4200000000000006E-2</v>
       </c>
       <c r="CI14">
         <v>0.6492</v>
@@ -4829,13 +4843,13 @@
         <v>9.8100000000000007E-2</v>
       </c>
       <c r="CS14">
-        <v>0.1009</v>
+        <v>9.4200000000000006E-2</v>
       </c>
       <c r="CT14">
-        <v>0.1</v>
+        <v>9.4200000000000006E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:98">
+    <row r="15" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>0.13541666666666666</v>
       </c>
@@ -5089,10 +5103,10 @@
         <v>9.4200000000000006E-2</v>
       </c>
       <c r="CG15">
-        <v>9.5100000000000004E-2</v>
+        <v>9.4200000000000006E-2</v>
       </c>
       <c r="CH15">
-        <v>9.5200000000000007E-2</v>
+        <v>9.4200000000000006E-2</v>
       </c>
       <c r="CI15">
         <v>0.80110000000000003</v>
@@ -5125,13 +5139,13 @@
         <v>9.8100000000000007E-2</v>
       </c>
       <c r="CS15">
-        <v>0.1019</v>
+        <v>9.4200000000000006E-2</v>
       </c>
       <c r="CT15">
-        <v>9.98E-2</v>
+        <v>9.4200000000000006E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:98">
+    <row r="16" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>0.14583333333333334</v>
       </c>
@@ -5385,10 +5399,10 @@
         <v>9.4E-2</v>
       </c>
       <c r="CG16">
-        <v>9.5100000000000004E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="CH16">
-        <v>9.5100000000000004E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="CI16">
         <v>0.95489999999999997</v>
@@ -5421,13 +5435,13 @@
         <v>9.9500000000000005E-2</v>
       </c>
       <c r="CS16">
-        <v>0.1033</v>
+        <v>9.4E-2</v>
       </c>
       <c r="CT16">
-        <v>9.9900000000000003E-2</v>
+        <v>9.4E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:98">
+    <row r="17" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>0.15625</v>
       </c>
@@ -5681,10 +5695,10 @@
         <v>9.4E-2</v>
       </c>
       <c r="CG17">
-        <v>9.5399999999999999E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="CH17">
-        <v>9.5000000000000001E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="CI17">
         <v>1.0337000000000001</v>
@@ -5717,13 +5731,13 @@
         <v>9.9299999999999999E-2</v>
       </c>
       <c r="CS17">
-        <v>0.1046</v>
+        <v>9.4E-2</v>
       </c>
       <c r="CT17">
-        <v>0.1</v>
+        <v>9.4E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:98">
+    <row r="18" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>0.16666666666666666</v>
       </c>
@@ -5977,10 +5991,10 @@
         <v>9.4E-2</v>
       </c>
       <c r="CG18">
-        <v>9.5200000000000007E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="CH18">
-        <v>9.5000000000000001E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="CI18">
         <v>1.0944</v>
@@ -6013,13 +6027,13 @@
         <v>9.7900000000000001E-2</v>
       </c>
       <c r="CS18">
-        <v>9.9599999999999994E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="CT18">
-        <v>9.9900000000000003E-2</v>
+        <v>9.4E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:98">
+    <row r="19" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>0.17708333333333334</v>
       </c>
@@ -6273,10 +6287,10 @@
         <v>9.4E-2</v>
       </c>
       <c r="CG19">
-        <v>9.5299999999999996E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="CH19">
-        <v>9.4799999999999995E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="CI19">
         <v>1.1581999999999999</v>
@@ -6309,13 +6323,13 @@
         <v>9.8400000000000001E-2</v>
       </c>
       <c r="CS19">
-        <v>9.8599999999999993E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="CT19">
-        <v>0.1018</v>
+        <v>9.4E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:98">
+    <row r="20" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>0.1875</v>
       </c>
@@ -6569,10 +6583,10 @@
         <v>9.4100000000000003E-2</v>
       </c>
       <c r="CG20">
-        <v>9.5699999999999993E-2</v>
+        <v>9.4100000000000003E-2</v>
       </c>
       <c r="CH20">
-        <v>9.4899999999999998E-2</v>
+        <v>9.4100000000000003E-2</v>
       </c>
       <c r="CI20">
         <v>1.2052</v>
@@ -6605,13 +6619,13 @@
         <v>9.9299999999999999E-2</v>
       </c>
       <c r="CS20">
-        <v>0.10050000000000001</v>
+        <v>9.4100000000000003E-2</v>
       </c>
       <c r="CT20">
-        <v>0.10009999999999999</v>
+        <v>9.4100000000000003E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:98">
+    <row r="21" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>0.19791666666666666</v>
       </c>
@@ -6865,10 +6879,10 @@
         <v>9.4E-2</v>
       </c>
       <c r="CG21">
-        <v>0.1154</v>
+        <v>9.4E-2</v>
       </c>
       <c r="CH21">
-        <v>0.4002</v>
+        <v>9.4E-2</v>
       </c>
       <c r="CI21">
         <v>1.2431000000000001</v>
@@ -6901,13 +6915,13 @@
         <v>0.1024</v>
       </c>
       <c r="CS21">
-        <v>0.18160000000000001</v>
+        <v>9.4E-2</v>
       </c>
       <c r="CT21">
-        <v>0.36830000000000002</v>
+        <v>9.4E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:98">
+    <row r="22" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>0.20833333333333334</v>
       </c>
@@ -7161,10 +7175,10 @@
         <v>9.4200000000000006E-2</v>
       </c>
       <c r="CG22">
-        <v>0.1111</v>
+        <v>9.4200000000000006E-2</v>
       </c>
       <c r="CH22">
-        <v>0.43369999999999997</v>
+        <v>9.4200000000000006E-2</v>
       </c>
       <c r="CI22">
         <v>1.2742</v>
@@ -7197,13 +7211,13 @@
         <v>0.1027</v>
       </c>
       <c r="CS22">
-        <v>0.1923</v>
+        <v>9.4200000000000006E-2</v>
       </c>
       <c r="CT22">
-        <v>0.40360000000000001</v>
+        <v>9.4200000000000006E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:98">
+    <row r="23" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>0.21875</v>
       </c>
@@ -7457,10 +7471,10 @@
         <v>9.4200000000000006E-2</v>
       </c>
       <c r="CG23">
-        <v>0.1085</v>
+        <v>9.4200000000000006E-2</v>
       </c>
       <c r="CH23">
-        <v>0.47560000000000002</v>
+        <v>9.4200000000000006E-2</v>
       </c>
       <c r="CI23">
         <v>1.2998000000000001</v>
@@ -7493,13 +7507,13 @@
         <v>9.8500000000000004E-2</v>
       </c>
       <c r="CS23">
-        <v>0.21149999999999999</v>
+        <v>9.4200000000000006E-2</v>
       </c>
       <c r="CT23">
-        <v>0.43980000000000002</v>
+        <v>9.4200000000000006E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:98">
+    <row r="24" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>0.22916666666666666</v>
       </c>
@@ -7753,10 +7767,10 @@
         <v>9.4700000000000006E-2</v>
       </c>
       <c r="CG24">
-        <v>0.1129</v>
+        <v>9.4700000000000006E-2</v>
       </c>
       <c r="CH24">
-        <v>0.52649999999999997</v>
+        <v>9.4700000000000006E-2</v>
       </c>
       <c r="CI24">
         <v>1.3201000000000001</v>
@@ -7789,13 +7803,13 @@
         <v>0.1048</v>
       </c>
       <c r="CS24">
-        <v>0.24129999999999999</v>
+        <v>9.4700000000000006E-2</v>
       </c>
       <c r="CT24">
-        <v>0.48720000000000002</v>
+        <v>9.4700000000000006E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:98">
+    <row r="25" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>0.23958333333333334</v>
       </c>
@@ -8049,10 +8063,10 @@
         <v>9.4299999999999995E-2</v>
       </c>
       <c r="CG25">
-        <v>0.1113</v>
+        <v>9.4299999999999995E-2</v>
       </c>
       <c r="CH25">
-        <v>0.59809999999999997</v>
+        <v>9.4299999999999995E-2</v>
       </c>
       <c r="CI25">
         <v>1.3404</v>
@@ -8085,13 +8099,13 @@
         <v>0.1037</v>
       </c>
       <c r="CS25">
-        <v>0.29210000000000003</v>
+        <v>9.4299999999999995E-2</v>
       </c>
       <c r="CT25">
-        <v>0.55669999999999997</v>
+        <v>9.4299999999999995E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:98">
+    <row r="26" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>0.25</v>
       </c>
@@ -8345,10 +8359,10 @@
         <v>9.4299999999999995E-2</v>
       </c>
       <c r="CG26">
-        <v>0.26150000000000001</v>
+        <v>9.4299999999999995E-2</v>
       </c>
       <c r="CH26">
-        <v>0.61250000000000004</v>
+        <v>9.4299999999999995E-2</v>
       </c>
       <c r="CI26">
         <v>1.3532</v>
@@ -8381,13 +8395,13 @@
         <v>9.98E-2</v>
       </c>
       <c r="CS26">
-        <v>0.35909999999999997</v>
+        <v>9.4299999999999995E-2</v>
       </c>
       <c r="CT26">
-        <v>0.59230000000000005</v>
+        <v>9.4299999999999995E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:98">
+    <row r="27" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>0.26041666666666669</v>
       </c>
@@ -8641,10 +8655,10 @@
         <v>9.4399999999999998E-2</v>
       </c>
       <c r="CG27">
-        <v>0.55289999999999995</v>
+        <v>9.4399999999999998E-2</v>
       </c>
       <c r="CH27">
-        <v>0.68089999999999995</v>
+        <v>9.4399999999999998E-2</v>
       </c>
       <c r="CI27">
         <v>1.3640000000000001</v>
@@ -8677,13 +8691,13 @@
         <v>9.9500000000000005E-2</v>
       </c>
       <c r="CS27">
-        <v>0.44479999999999997</v>
+        <v>9.4399999999999998E-2</v>
       </c>
       <c r="CT27">
-        <v>0.60409999999999997</v>
+        <v>9.4399999999999998E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:98">
+    <row r="28" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>0.27083333333333331</v>
       </c>
@@ -8937,10 +8951,10 @@
         <v>9.4500000000000001E-2</v>
       </c>
       <c r="CG28">
-        <v>0.60640000000000005</v>
+        <v>9.4500000000000001E-2</v>
       </c>
       <c r="CH28">
-        <v>0.74309999999999998</v>
+        <v>9.4500000000000001E-2</v>
       </c>
       <c r="CI28">
         <v>1.3704000000000001</v>
@@ -8973,13 +8987,13 @@
         <v>0.1052</v>
       </c>
       <c r="CS28">
-        <v>0.52829999999999999</v>
+        <v>9.4500000000000001E-2</v>
       </c>
       <c r="CT28">
-        <v>0.6431</v>
+        <v>9.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:98">
+    <row r="29" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>0.28125</v>
       </c>
@@ -9233,10 +9247,10 @@
         <v>9.4500000000000001E-2</v>
       </c>
       <c r="CG29">
-        <v>0.65449999999999997</v>
+        <v>9.4500000000000001E-2</v>
       </c>
       <c r="CH29">
-        <v>0.76759999999999995</v>
+        <v>9.4500000000000001E-2</v>
       </c>
       <c r="CI29">
         <v>1.3738999999999999</v>
@@ -9269,13 +9283,13 @@
         <v>9.8000000000000004E-2</v>
       </c>
       <c r="CS29">
-        <v>0.58150000000000002</v>
+        <v>9.4500000000000001E-2</v>
       </c>
       <c r="CT29">
-        <v>0.69199999999999995</v>
+        <v>9.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:98">
+    <row r="30" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>0.29166666666666669</v>
       </c>
@@ -9529,10 +9543,10 @@
         <v>9.4600000000000004E-2</v>
       </c>
       <c r="CG30">
-        <v>0.70209999999999995</v>
+        <v>9.4600000000000004E-2</v>
       </c>
       <c r="CH30">
-        <v>0.77900000000000003</v>
+        <v>9.4600000000000004E-2</v>
       </c>
       <c r="CI30">
         <v>1.3774</v>
@@ -9565,13 +9579,13 @@
         <v>9.8299999999999998E-2</v>
       </c>
       <c r="CS30">
-        <v>0.62439999999999996</v>
+        <v>9.4600000000000004E-2</v>
       </c>
       <c r="CT30">
-        <v>0.71640000000000004</v>
+        <v>9.4600000000000004E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:98">
+    <row r="31" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>0.30208333333333331</v>
       </c>
@@ -9825,10 +9839,10 @@
         <v>9.4700000000000006E-2</v>
       </c>
       <c r="CG31">
-        <v>0.74770000000000003</v>
+        <v>9.4700000000000006E-2</v>
       </c>
       <c r="CH31">
-        <v>0.79820000000000002</v>
+        <v>9.4700000000000006E-2</v>
       </c>
       <c r="CI31">
         <v>1.3791</v>
@@ -9861,13 +9875,13 @@
         <v>9.8000000000000004E-2</v>
       </c>
       <c r="CS31">
-        <v>0.69520000000000004</v>
+        <v>9.4700000000000006E-2</v>
       </c>
       <c r="CT31">
-        <v>0.73250000000000004</v>
+        <v>9.4700000000000006E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:98">
+    <row r="32" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>0.3125</v>
       </c>
@@ -10121,10 +10135,10 @@
         <v>9.4700000000000006E-2</v>
       </c>
       <c r="CG32">
-        <v>0.79479999999999995</v>
+        <v>9.4700000000000006E-2</v>
       </c>
       <c r="CH32">
-        <v>0.84240000000000004</v>
+        <v>9.4700000000000006E-2</v>
       </c>
       <c r="CI32">
         <v>1.3791</v>
@@ -10157,13 +10171,13 @@
         <v>9.8000000000000004E-2</v>
       </c>
       <c r="CS32">
-        <v>0.73399999999999999</v>
+        <v>9.4700000000000006E-2</v>
       </c>
       <c r="CT32">
-        <v>0.77200000000000002</v>
+        <v>9.4700000000000006E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:98">
+    <row r="33" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>0.32291666666666669</v>
       </c>
@@ -10417,10 +10431,10 @@
         <v>9.4799999999999995E-2</v>
       </c>
       <c r="CG33">
-        <v>0.77129999999999999</v>
+        <v>9.4799999999999995E-2</v>
       </c>
       <c r="CH33">
-        <v>0.86850000000000005</v>
+        <v>9.4799999999999995E-2</v>
       </c>
       <c r="CI33">
         <v>1.3796999999999999</v>
@@ -10453,13 +10467,13 @@
         <v>9.8199999999999996E-2</v>
       </c>
       <c r="CS33">
-        <v>0.77510000000000001</v>
+        <v>9.4799999999999995E-2</v>
       </c>
       <c r="CT33">
-        <v>0.7994</v>
+        <v>9.4799999999999995E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:98">
+    <row r="34" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>0.33333333333333331</v>
       </c>
@@ -10713,10 +10727,10 @@
         <v>9.4799999999999995E-2</v>
       </c>
       <c r="CG34">
-        <v>0.76359999999999995</v>
+        <v>9.4799999999999995E-2</v>
       </c>
       <c r="CH34">
-        <v>0.86919999999999997</v>
+        <v>9.4799999999999995E-2</v>
       </c>
       <c r="CI34">
         <v>1.3778999999999999</v>
@@ -10749,13 +10763,13 @@
         <v>9.8100000000000007E-2</v>
       </c>
       <c r="CS34">
-        <v>0.77549999999999997</v>
+        <v>9.4799999999999995E-2</v>
       </c>
       <c r="CT34">
-        <v>0.80469999999999997</v>
+        <v>9.4799999999999995E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:98">
+    <row r="35" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>0.34375</v>
       </c>
@@ -11009,10 +11023,10 @@
         <v>9.4899999999999998E-2</v>
       </c>
       <c r="CG35">
-        <v>0.74309999999999998</v>
+        <v>9.4899999999999998E-2</v>
       </c>
       <c r="CH35">
-        <v>0.85680000000000001</v>
+        <v>9.4899999999999998E-2</v>
       </c>
       <c r="CI35">
         <v>1.3763000000000001</v>
@@ -11045,13 +11059,13 @@
         <v>9.8299999999999998E-2</v>
       </c>
       <c r="CS35">
-        <v>0.78790000000000004</v>
+        <v>9.4899999999999998E-2</v>
       </c>
       <c r="CT35">
-        <v>0.80840000000000001</v>
+        <v>9.4899999999999998E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:98">
+    <row r="36" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>0.35416666666666669</v>
       </c>
@@ -11305,10 +11319,10 @@
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="CG36">
-        <v>0.75329999999999997</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="CH36">
-        <v>0.82230000000000003</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="CI36">
         <v>1.3711</v>
@@ -11341,13 +11355,13 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="CS36">
-        <v>0.80230000000000001</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="CT36">
-        <v>0.80920000000000003</v>
+        <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:98">
+    <row r="37" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>0.36458333333333331</v>
       </c>
@@ -11601,10 +11615,10 @@
         <v>9.5500000000000002E-2</v>
       </c>
       <c r="CG37">
-        <v>0.75</v>
+        <v>9.5500000000000002E-2</v>
       </c>
       <c r="CH37">
-        <v>0.80359999999999998</v>
+        <v>9.5500000000000002E-2</v>
       </c>
       <c r="CI37">
         <v>1.3682000000000001</v>
@@ -11637,13 +11651,13 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="CS37">
-        <v>0.79690000000000005</v>
+        <v>9.5500000000000002E-2</v>
       </c>
       <c r="CT37">
-        <v>0.8034</v>
+        <v>9.5500000000000002E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:98">
+    <row r="38" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>0.375</v>
       </c>
@@ -11897,10 +11911,10 @@
         <v>9.5200000000000007E-2</v>
       </c>
       <c r="CG38">
-        <v>0.72809999999999997</v>
+        <v>9.5200000000000007E-2</v>
       </c>
       <c r="CH38">
-        <v>0.76929999999999998</v>
+        <v>9.5200000000000007E-2</v>
       </c>
       <c r="CI38">
         <v>1.3636999999999999</v>
@@ -11933,13 +11947,13 @@
         <v>9.8400000000000001E-2</v>
       </c>
       <c r="CS38">
-        <v>0.78110000000000002</v>
+        <v>9.5200000000000007E-2</v>
       </c>
       <c r="CT38">
-        <v>0.80230000000000001</v>
+        <v>9.5200000000000007E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:98">
+    <row r="39" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>0.38541666666666669</v>
       </c>
@@ -12193,10 +12207,10 @@
         <v>9.5299999999999996E-2</v>
       </c>
       <c r="CG39">
-        <v>0.73640000000000005</v>
+        <v>9.5299999999999996E-2</v>
       </c>
       <c r="CH39">
-        <v>0.77449999999999997</v>
+        <v>9.5299999999999996E-2</v>
       </c>
       <c r="CI39">
         <v>1.3596999999999999</v>
@@ -12229,13 +12243,13 @@
         <v>9.8400000000000001E-2</v>
       </c>
       <c r="CS39">
-        <v>0.7853</v>
+        <v>9.5299999999999996E-2</v>
       </c>
       <c r="CT39">
-        <v>0.79669999999999996</v>
+        <v>9.5299999999999996E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:98">
+    <row r="40" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>0.39583333333333331</v>
       </c>
@@ -12489,10 +12503,10 @@
         <v>9.5399999999999999E-2</v>
       </c>
       <c r="CG40">
-        <v>0.72360000000000002</v>
+        <v>9.5399999999999999E-2</v>
       </c>
       <c r="CH40">
-        <v>0.76529999999999998</v>
+        <v>9.5399999999999999E-2</v>
       </c>
       <c r="CI40">
         <v>1.3548</v>
@@ -12525,13 +12539,13 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="CS40">
-        <v>0.78639999999999999</v>
+        <v>9.5399999999999999E-2</v>
       </c>
       <c r="CT40">
-        <v>0.79820000000000002</v>
+        <v>9.5399999999999999E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:98">
+    <row r="41" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>0.40625</v>
       </c>
@@ -12785,10 +12799,10 @@
         <v>9.5500000000000002E-2</v>
       </c>
       <c r="CG41">
-        <v>0.72470000000000001</v>
+        <v>9.5500000000000002E-2</v>
       </c>
       <c r="CH41">
-        <v>0.76019999999999999</v>
+        <v>9.5500000000000002E-2</v>
       </c>
       <c r="CI41">
         <v>1.3487</v>
@@ -12821,13 +12835,13 @@
         <v>9.8900000000000002E-2</v>
       </c>
       <c r="CS41">
-        <v>0.76759999999999995</v>
+        <v>9.5500000000000002E-2</v>
       </c>
       <c r="CT41">
-        <v>0.80910000000000004</v>
+        <v>9.5500000000000002E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:98">
+    <row r="42" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>0.41666666666666669</v>
       </c>
@@ -13081,10 +13095,10 @@
         <v>9.5600000000000004E-2</v>
       </c>
       <c r="CG42">
-        <v>0.70779999999999998</v>
+        <v>9.5600000000000004E-2</v>
       </c>
       <c r="CH42">
-        <v>0.75029999999999997</v>
+        <v>9.5600000000000004E-2</v>
       </c>
       <c r="CI42">
         <v>1.343</v>
@@ -13117,10 +13131,10 @@
         <v>9.9299999999999999E-2</v>
       </c>
       <c r="CS42">
-        <v>0.78080000000000005</v>
+        <v>9.5600000000000004E-2</v>
       </c>
       <c r="CT42">
-        <v>0.81320000000000003</v>
+        <v>9.5600000000000004E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>